<commit_message>
working on beta release
</commit_message>
<xml_diff>
--- a/app/application/views/rpt/ru/LedgerPayments.xlsx
+++ b/app/application/views/rpt/ru/LedgerPayments.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\wamp\www\isell3\application\views\rpt\ru\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505"/>
   </bookViews>
   <sheets>
     <sheet name="Акт звіряння" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -93,9 +88,6 @@
   </si>
   <si>
     <t>Итого</t>
-  </si>
-  <si>
-    <t>Сальдо на {$v-&gt;localDate} г.</t>
   </si>
   <si>
     <t>ПОДПИСИ СТОРОН :</t>
@@ -142,9 +134,6 @@
     <t>Сумма</t>
   </si>
   <si>
-    <t xml:space="preserve"> {$v-&gt;spell}</t>
-  </si>
-  <si>
     <r>
       <t>Руководитель___________</t>
     </r>
@@ -160,12 +149,18 @@
       <t>{$v-&gt;director_name}</t>
     </r>
   </si>
+  <si>
+    <t>Сальдо на {$v-&gt;flocalDate} г.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> {$v-&gt;spell} </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -211,6 +206,22 @@
       <family val="2"/>
       <charset val="204"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF008000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -247,64 +258,70 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -374,7 +391,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -409,7 +426,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -620,8 +637,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23:G23"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19:G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -634,330 +651,330 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
     </row>
     <row r="2" spans="1:7" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
     </row>
     <row r="5" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
+      <c r="B5" s="21"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
     </row>
     <row r="6" spans="1:7" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
     </row>
     <row r="7" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
     </row>
     <row r="8" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
+      <c r="B8" s="19"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="19"/>
     </row>
     <row r="9" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
     </row>
     <row r="10" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7" t="s">
+      <c r="E10" s="18"/>
+      <c r="F10" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="G10" s="7"/>
+      <c r="G10" s="18"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="9"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="8" t="s">
+      <c r="A11" s="22"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="E11" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F11" s="8" t="s">
+      <c r="F11" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="G11" s="8" t="s">
+      <c r="G11" s="3" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="8">
+      <c r="A12" s="3">
         <v>1</v>
       </c>
-      <c r="B12" s="8">
+      <c r="B12" s="3">
         <v>2</v>
       </c>
-      <c r="C12" s="8">
+      <c r="C12" s="3">
         <v>3</v>
       </c>
-      <c r="D12" s="8">
+      <c r="D12" s="3">
         <v>4</v>
       </c>
-      <c r="E12" s="8">
+      <c r="E12" s="3">
         <v>5</v>
       </c>
-      <c r="F12" s="8">
+      <c r="F12" s="3">
         <v>6</v>
       </c>
-      <c r="G12" s="8">
+      <c r="G12" s="3">
         <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A13" s="12" t="s">
+      <c r="A13" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="17"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="9"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+    </row>
+    <row r="15" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A15" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="17"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+    </row>
+    <row r="16" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A16" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="20" t="s">
+      <c r="B16" s="17"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="E13" s="18"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="E14" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="E15" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="E16" s="17"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="13"/>
-      <c r="B17" s="13"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
+      <c r="A17" s="6"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
     </row>
     <row r="18" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="16" t="str">
+      <c r="A18" s="14" t="str">
         <f>"Сальдо в пользу "&amp;IF(D16&gt;0,A22,D22)</f>
         <v>Сальдо в пользу {$v-&gt;a-&gt;company_name}</v>
       </c>
-      <c r="B18" s="16"/>
-      <c r="C18" s="16"/>
-      <c r="D18" s="16"/>
-      <c r="E18" s="16"/>
-      <c r="F18" s="16"/>
-      <c r="G18" s="16"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
     </row>
     <row r="19" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A19" s="16" t="s">
+      <c r="A19" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" s="14"/>
+      <c r="C19" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D19" s="16"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="16"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="6"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" s="14"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+    </row>
+    <row r="22" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A22" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" s="16"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="E22" s="16"/>
+      <c r="F22" s="16"/>
+      <c r="G22" s="16"/>
+    </row>
+    <row r="23" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A23" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="B19" s="16"/>
-      <c r="C19" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="D19" s="19"/>
-      <c r="E19" s="19"/>
-      <c r="F19" s="19"/>
-      <c r="G19" s="19"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" s="13"/>
-      <c r="B20" s="13"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" s="16" t="s">
+      <c r="B23" s="14"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="14"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="6"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+    </row>
+    <row r="25" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A25" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25" s="14"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="B21" s="16"/>
-      <c r="C21" s="16"/>
-      <c r="D21" s="16"/>
-      <c r="E21" s="16"/>
-      <c r="F21" s="16"/>
-      <c r="G21" s="16"/>
-    </row>
-    <row r="22" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A22" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="B22" s="19"/>
-      <c r="C22" s="19"/>
-      <c r="D22" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="E22" s="19"/>
-      <c r="F22" s="19"/>
-      <c r="G22" s="19"/>
-    </row>
-    <row r="23" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A23" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="B23" s="16"/>
-      <c r="C23" s="16"/>
-      <c r="D23" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="E23" s="16"/>
-      <c r="F23" s="16"/>
-      <c r="G23" s="16"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" s="13"/>
-      <c r="B24" s="13"/>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="14"/>
-      <c r="G24" s="14"/>
-    </row>
-    <row r="25" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A25" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="B25" s="16"/>
-      <c r="C25" s="16"/>
-      <c r="D25" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="E25" s="16"/>
-      <c r="F25" s="16"/>
-      <c r="G25" s="16"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="14"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A26" s="13"/>
-      <c r="B26" s="13"/>
-      <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
+      <c r="A26" s="6"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B27" s="15"/>
       <c r="C27" s="15"/>
       <c r="D27" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E27" s="15"/>
       <c r="F27" s="15"/>
@@ -965,6 +982,23 @@
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="A5:E5"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A6:E6"/>
+    <mergeCell ref="A7:E7"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="A8:G8"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A18:G18"/>
+    <mergeCell ref="F10:G10"/>
     <mergeCell ref="A25:C25"/>
     <mergeCell ref="D25:G25"/>
     <mergeCell ref="A27:C27"/>
@@ -976,23 +1010,6 @@
     <mergeCell ref="D22:G22"/>
     <mergeCell ref="A23:C23"/>
     <mergeCell ref="D23:G23"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="A18:G18"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="A6:E6"/>
-    <mergeCell ref="A7:E7"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="A8:G8"/>
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="A5:E5"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="A1:G1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>

</xml_diff>